<commit_message>
Added full version of the Penman Monteith calculator
</commit_message>
<xml_diff>
--- a/tools/PenmanMonteithCalculator.xlsx
+++ b/tools/PenmanMonteithCalculator.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sherzodr\Documents\eclipse-workspace\agriclimuz\tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{589018A4-215B-436C-8E19-D25A6B6B7213}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8D089A0-DD68-46FB-920D-26F5780D23E4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="447" xr2:uid="{49EFD1A0-30FE-4D89-822D-832008CA9853}"/>
   </bookViews>
@@ -1737,6 +1737,10 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyProtection="1"/>
+    <xf numFmtId="43" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1747,10 +1751,6 @@
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="43" fontId="7" fillId="2" borderId="1" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -1759,44 +1759,6 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="33">
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <protection locked="0" hidden="0"/>
-    </dxf>
     <dxf>
       <font>
         <strike val="0"/>
@@ -2458,6 +2420,44 @@
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <protection locked="1" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <protection locked="0" hidden="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3681,78 +3681,78 @@
     <tableColumn id="2" xr3:uid="{0343CEB4-F964-43A1-BDB3-F2FEF6A7C729}" name="Тмин_x000a_(°С)" dataDxfId="29" dataCellStyle="Comma"/>
     <tableColumn id="3" xr3:uid="{9BD57D35-89FF-4084-9359-B7214AD803FE}" name="Тмакс_x000a_(°С)" dataDxfId="28" dataCellStyle="Comma"/>
     <tableColumn id="6" xr3:uid="{41B592D5-95B1-44E5-A64B-BDDC9D6D5BCA}" name="Шамол_x000a_(м/с)" dataDxfId="27" dataCellStyle="Comma"/>
-    <tableColumn id="20" xr3:uid="{2ABE4840-178F-4818-A24E-0EF1AE56B41F}" name="Қуёшли соат" dataDxfId="1" dataCellStyle="Comma"/>
-    <tableColumn id="27" xr3:uid="{026FEEB6-B796-4EDB-9611-B4B15F3B7F32}" name="Радиация_x000a_(MJ/м2/к)" dataDxfId="0" dataCellStyle="Comma"/>
-    <tableColumn id="21" xr3:uid="{A535BD23-5121-4397-AC1B-E39E70B75654}" name="Tmean" dataDxfId="26" dataCellStyle="Comma">
+    <tableColumn id="20" xr3:uid="{2ABE4840-178F-4818-A24E-0EF1AE56B41F}" name="Қуёшли соат" dataDxfId="26" dataCellStyle="Comma"/>
+    <tableColumn id="27" xr3:uid="{026FEEB6-B796-4EDB-9611-B4B15F3B7F32}" name="Радиация_x000a_(MJ/м2/к)" dataDxfId="25" dataCellStyle="Comma"/>
+    <tableColumn id="21" xr3:uid="{A535BD23-5121-4397-AC1B-E39E70B75654}" name="Tmean" dataDxfId="24" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF( AND(ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]]), ISNUMBER(EToTable[[#This Row],[Тмакс
 (°С)]])), (EToTable[[#This Row],[Тмин
 (°С)]]+EToTable[[#This Row],[Тмакс
 (°С)]])/2, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="4" xr3:uid="{28F03338-A80A-46CA-90C2-3EE3FE3141B5}" name="Tdew" dataDxfId="25" dataCellStyle="Comma">
+    <tableColumn id="4" xr3:uid="{28F03338-A80A-46CA-90C2-3EE3FE3141B5}" name="Tdew" dataDxfId="23" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]])), EToTable[[#This Row],[Тмин
 (°С)]]-TdewSubtract, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="22" xr3:uid="{72ED62CD-F87B-4F4E-8A95-741E4046A8D2}" name="J" dataDxfId="24" dataCellStyle="Comma">
+    <tableColumn id="22" xr3:uid="{72ED62CD-F87B-4F4E-8A95-741E4046A8D2}" name="J" dataDxfId="22" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Сана]]), _xlfn.DAYS(EToTable[[#This Row],[Сана]], "1/1/" &amp; YEAR(EToTable[[#This Row],[Сана]])) + 1, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="34" xr3:uid="{91194067-8744-4547-AC20-6D98CC22490B}" name="P" dataDxfId="23" dataCellStyle="Comma">
+    <tableColumn id="34" xr3:uid="{91194067-8744-4547-AC20-6D98CC22490B}" name="P" dataDxfId="21" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(Altitude), ISNUMBER(EToTable[[#This Row],[Сана]])),  ROUND(101.3 * POWER( (293-0.0065 * Altitude) / 293, 5.26), 2), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="33" xr3:uid="{29003213-DC54-4480-A40A-0FC6ABBE0369}" name="γ" dataDxfId="22" dataCellStyle="Comma">
+    <tableColumn id="33" xr3:uid="{29003213-DC54-4480-A40A-0FC6ABBE0369}" name="γ" dataDxfId="20" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[P]]), (Cp * EToTable[[#This Row],[P]]) / (0.622 * 2.45), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="19" xr3:uid="{0E062F52-C43F-4056-A51C-394BD475D85F}" name="Δ" dataDxfId="21" dataCellStyle="Comma">
+    <tableColumn id="19" xr3:uid="{0E062F52-C43F-4056-A51C-394BD475D85F}" name="Δ" dataDxfId="19" dataCellStyle="Comma">
       <calculatedColumnFormula>IF( ISNUMBER(EToTable[[#This Row],[Tmean]]), ROUND((4098 * (0.6108 * EXP((17.27 * EToTable[[#This Row],[Tmean]]) / (EToTable[[#This Row],[Tmean]] + 237.3)))) / ((EToTable[[#This Row],[Tmean]] + 237.3) ^ 2), 4), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="18" xr3:uid="{76882BE6-D768-4B05-B6A0-08F20B3C673F}" name="δ (rad)" dataDxfId="20" dataCellStyle="Comma">
+    <tableColumn id="18" xr3:uid="{76882BE6-D768-4B05-B6A0-08F20B3C673F}" name="δ (rad)" dataDxfId="18" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[J]]), 0.409  * SIN( (2*PI()/365) * EToTable[[#This Row],[J]] - 1.39), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="17" xr3:uid="{A21CD0BD-4854-4025-84DD-72F473757E0B}" name="dr" dataDxfId="19" dataCellStyle="Comma">
+    <tableColumn id="17" xr3:uid="{A21CD0BD-4854-4025-84DD-72F473757E0B}" name="dr" dataDxfId="17" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[J]]), ROUND(1+0.033 * COS( (2*PI()/365) * EToTable[[#This Row],[J]]), 4), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="23" xr3:uid="{CE40DA70-CBFE-48A6-AC64-4663E945330A}" name="φ" dataDxfId="18" dataCellStyle="Comma">
+    <tableColumn id="23" xr3:uid="{CE40DA70-CBFE-48A6-AC64-4663E945330A}" name="φ" dataDxfId="16" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(Latitude), ISNUMBER(EToTable[[#This Row],[Сана]])), ROUND((Latitude / 180) * PI(), 3), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="16" xr3:uid="{F874822E-F3EF-4453-A539-2D54B0627751}" name="ωs" dataDxfId="17" dataCellStyle="Comma">
+    <tableColumn id="16" xr3:uid="{F874822E-F3EF-4453-A539-2D54B0627751}" name="ωs" dataDxfId="15" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[φ]]), ISNUMBER(EToTable[[#This Row],[δ (rad)]])), ACOS( - 1 * TAN(EToTable[[#This Row],[φ]]) * TAN(EToTable[[#This Row],[δ (rad)]])), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="15" xr3:uid="{8FD74915-A745-43A9-912D-0965AB100C05}" name="Ra" dataDxfId="16" dataCellStyle="Comma">
+    <tableColumn id="15" xr3:uid="{8FD74915-A745-43A9-912D-0965AB100C05}" name="Ra" dataDxfId="14" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(AND(ISNUMBER(EToTable[[#This Row],[ωs]]), ISNUMBER(EToTable[[#This Row],[dr]])), ((24 * 60) / 3.1416) * 0.082 * EToTable[[#This Row],[dr]] * ((EToTable[[#This Row],[ωs]] * SIN(EToTable[[#This Row],[φ]]) * SIN(EToTable[[#This Row],[δ (rad)]])) + (COS(EToTable[[#This Row],[φ]]) * COS(EToTable[[#This Row],[δ (rad)]]) * SIN(EToTable[[#This Row],[ωs]]))), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="14" xr3:uid="{BD9990DB-8992-4E9A-893D-DCB28C028665}" name="N" dataDxfId="15" dataCellStyle="Comma">
+    <tableColumn id="14" xr3:uid="{BD9990DB-8992-4E9A-893D-DCB28C028665}" name="N" dataDxfId="13" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(ISNUMBER(EToTable[[#This Row],[ωs]]), ( 24 / PI()) * EToTable[[#This Row],[ωs]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="13" xr3:uid="{017B251A-16BB-4EF8-B942-DB81DD2D951E}" name="e° (Tmin)" dataDxfId="14" dataCellStyle="Comma">
+    <tableColumn id="13" xr3:uid="{017B251A-16BB-4EF8-B942-DB81DD2D951E}" name="e° (Tmin)" dataDxfId="12" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]]), 0.6108 * EXP( 17.27 * EToTable[[#This Row],[Тмин
 (°С)]] / (EToTable[[#This Row],[Тмин
 (°С)]]+237.3)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="12" xr3:uid="{0488585F-8BE0-4299-A580-08C3CBFA1E59}" name="e° (Tmax)" dataDxfId="13" dataCellStyle="Comma">
+    <tableColumn id="12" xr3:uid="{0488585F-8BE0-4299-A580-08C3CBFA1E59}" name="e° (Tmax)" dataDxfId="11" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Тмакс
 (°С)]]), 0.6108 * EXP( 17.27 * EToTable[[#This Row],[Тмакс
 (°С)]] / (EToTable[[#This Row],[Тмакс
 (°С)]]+237.3)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="11" xr3:uid="{DC14E8C3-BA59-4195-BBB3-8106DA52F7F7}" name="es" dataDxfId="12" dataCellStyle="Comma">
+    <tableColumn id="11" xr3:uid="{DC14E8C3-BA59-4195-BBB3-8106DA52F7F7}" name="es" dataDxfId="10" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[e° (Tmin)]]), ISNUMBER(EToTable[[#This Row],[e° (Tmax)]])), (EToTable[[#This Row],[e° (Tmax)]]+EToTable[[#This Row],[e° (Tmin)]])/2, "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="24" xr3:uid="{57F5EDAF-2374-49FE-9B64-AB6BBD822583}" name="e° (Tdew)" dataDxfId="11" dataCellStyle="Comma">
+    <tableColumn id="24" xr3:uid="{57F5EDAF-2374-49FE-9B64-AB6BBD822583}" name="e° (Tdew)" dataDxfId="9" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Tdew]]), 0.6108 * EXP( 17.27 * (EToTable[[#This Row],[Tdew]]) / (EToTable[[#This Row],[Tdew]]+237.3)), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="10" xr3:uid="{627FA355-70D4-4E6A-A764-1C5826BB96A2}" name="ea" dataDxfId="10" dataCellStyle="Comma">
+    <tableColumn id="10" xr3:uid="{627FA355-70D4-4E6A-A764-1C5826BB96A2}" name="ea" dataDxfId="8" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> EToTable[[#This Row],[e° (Tdew)]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="9" xr3:uid="{9E010230-CD5B-42D5-8FA2-D17763D5D2AC}" name="es - ea" dataDxfId="9" dataCellStyle="Comma">
+    <tableColumn id="9" xr3:uid="{9E010230-CD5B-42D5-8FA2-D17763D5D2AC}" name="es - ea" dataDxfId="7" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[es]]), ISNUMBER(EToTable[[#This Row],[ea]])), EToTable[[#This Row],[es]]-EToTable[[#This Row],[ea]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="8" xr3:uid="{5EAFCF03-F1FE-46B0-8665-1FD5A41B6C5E}" name="Rso" dataDxfId="8" dataCellStyle="Comma">
+    <tableColumn id="8" xr3:uid="{5EAFCF03-F1FE-46B0-8665-1FD5A41B6C5E}" name="Rso" dataDxfId="6" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Ra]]), (as+bs)*EToTable[[#This Row],[Ra]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="26" xr3:uid="{42FE00EA-A686-4C84-8B12-E62382B4D2E8}" name="Rs" dataDxfId="7" dataCellStyle="Comma">
+    <tableColumn id="26" xr3:uid="{42FE00EA-A686-4C84-8B12-E62382B4D2E8}" name="Rs" dataDxfId="5" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]]), ISNUMBER(EToTable[[#This Row],[Тмакс
 (°С)]])), IF(ISNUMBER(EToTable[[#This Row],[Радиация
@@ -3761,10 +3761,10 @@
 (°С)]]-EToTable[[#This Row],[Тмин
 (°С)]] ) * EToTable[[#This Row],[Ra]] ) ), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="25" xr3:uid="{D2310C7E-B446-4405-BEDC-9493BA3EA074}" name="Rns" dataDxfId="6" dataCellStyle="Comma">
+    <tableColumn id="25" xr3:uid="{D2310C7E-B446-4405-BEDC-9493BA3EA074}" name="Rns" dataDxfId="4" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Rs]]), (1-albedo)*EToTable[[#This Row],[Rs]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="28" xr3:uid="{246D79AE-5292-4B8C-8FD4-BAB9ABA083D4}" name="Rnl" dataDxfId="5" dataCellStyle="Comma">
+    <tableColumn id="28" xr3:uid="{246D79AE-5292-4B8C-8FD4-BAB9ABA083D4}" name="Rnl" dataDxfId="3" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[Rso]]), ISNUMBER(EToTable[[#This Row],[ea]]), ISNUMBER(EToTable[[#This Row],[Rs]])), StefanBoltzmann *
 (( POWER(EToTable[[#This Row],[Тмакс
 (°С)]]+273.16, 4) + POWER( EToTable[[#This Row],[Тмин
@@ -3772,10 +3772,10 @@
 (0.34 - 0.14 * SQRT(EToTable[[#This Row],[ea]])) *
 ( (1.35 * EToTable[[#This Row],[Rs]]/EToTable[[#This Row],[Rso]]) - 0.35), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="29" xr3:uid="{422888C5-5DC5-4D70-B7D8-B3F6A9456433}" name="Rn" dataDxfId="4" dataCellStyle="Comma">
+    <tableColumn id="29" xr3:uid="{422888C5-5DC5-4D70-B7D8-B3F6A9456433}" name="Rn" dataDxfId="2" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(AND(ISNUMBER(EToTable[[#This Row],[Rns]]), ISNUMBER(EToTable[[#This Row],[Rnl]])), EToTable[[#This Row],[Rns]]-EToTable[[#This Row],[Rnl]], "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="30" xr3:uid="{9B0CC101-DA7D-4460-9098-E50E3E62164F}" name="u2" dataDxfId="3" dataCellStyle="Comma">
+    <tableColumn id="30" xr3:uid="{9B0CC101-DA7D-4460-9098-E50E3E62164F}" name="u2" dataDxfId="1" dataCellStyle="Comma">
       <calculatedColumnFormula>IF(ISNUMBER(EToTable[[#This Row],[Сана]]), IF(ISNUMBER(EToTable[[#This Row],[Шамол
 (м/с)]]),
      IF(AnemometerHeight=2, MAX(EToTable[[#This Row],[Шамол
@@ -3784,7 +3784,7 @@
 (м/с)]] * 4.87 / LN(67.8 * AnemometerHeight - 5.42), 0.5)
 ), u2_default), "")</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="7" xr3:uid="{F7425A71-C167-48A6-930B-0E92D3200E4B}" name=" ETO_x000a_(мм)" dataDxfId="2" dataCellStyle="Comma">
+    <tableColumn id="7" xr3:uid="{F7425A71-C167-48A6-930B-0E92D3200E4B}" name=" ETO_x000a_(мм)" dataDxfId="0" dataCellStyle="Comma">
       <calculatedColumnFormula xml:space="preserve"> IF(AND(ISNUMBER(Latitude), ISNUMBER(Altitude), ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]]), ISNUMBER(EToTable[[#This Row],[Тмакс
 (°С)]])),   ((0.408 * EToTable[[#This Row],[Δ]] * (EToTable[[#This Row],[Rn]]-0))
@@ -4099,7 +4099,7 @@
       <pane xSplit="3" ySplit="9" topLeftCell="D10" activePane="bottomRight" state="frozenSplit"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="D2" sqref="D2:F2"/>
+      <selection pane="bottomRight" activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -4145,14 +4145,14 @@
       <c r="AE1" s="6"/>
     </row>
     <row r="2" spans="1:35" customFormat="1" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="53" t="s">
+      <c r="A2" s="54" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="53"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
+      <c r="B2" s="54"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="7"/>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
@@ -4247,7 +4247,7 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4" s="6"/>
-      <c r="AE4" s="56"/>
+      <c r="AE4" s="53"/>
       <c r="AG4" s="51"/>
       <c r="AH4" s="52"/>
     </row>
@@ -4429,35 +4429,29 @@
       </c>
     </row>
     <row r="10" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A10" s="20">
-        <v>44297</v>
-      </c>
-      <c r="B10" s="21">
-        <v>21.1</v>
-      </c>
-      <c r="C10" s="22">
-        <v>31.2</v>
-      </c>
+      <c r="A10" s="20"/>
+      <c r="B10" s="21"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="32"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
-      <c r="G10" s="42">
+      <c r="G10" s="42" t="str">
         <f xml:space="preserve"> IF( AND(ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]]), ISNUMBER(EToTable[[#This Row],[Тмакс
 (°С)]])), (EToTable[[#This Row],[Тмин
 (°С)]]+EToTable[[#This Row],[Тмакс
 (°С)]])/2, "")</f>
-        <v>26.15</v>
-      </c>
-      <c r="H10" s="42">
+        <v/>
+      </c>
+      <c r="H10" s="42" t="str">
         <f>IF(AND(ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]])), EToTable[[#This Row],[Тмин
 (°С)]]-TdewSubtract, "")</f>
-        <v>19.100000000000001</v>
-      </c>
-      <c r="I10" s="35">
+        <v/>
+      </c>
+      <c r="I10" s="35" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[Сана]]), _xlfn.DAYS(EToTable[[#This Row],[Сана]], "1/1/" &amp; YEAR(EToTable[[#This Row],[Сана]])) + 1, "")</f>
-        <v>101</v>
+        <v/>
       </c>
       <c r="J10" s="28" t="str">
         <f>IF(AND(ISNUMBER(Altitude), ISNUMBER(EToTable[[#This Row],[Сана]])),  ROUND(101.3 * POWER( (293-0.0065 * Altitude) / 293, 5.26), 2), "")</f>
@@ -4467,17 +4461,17 @@
         <f>IF(ISNUMBER(EToTable[[#This Row],[P]]), (Cp * EToTable[[#This Row],[P]]) / (0.622 * 2.45), "")</f>
         <v/>
       </c>
-      <c r="L10" s="29">
+      <c r="L10" s="29" t="str">
         <f>IF( ISNUMBER(EToTable[[#This Row],[Tmean]]), ROUND((4098 * (0.6108 * EXP((17.27 * EToTable[[#This Row],[Tmean]]) / (EToTable[[#This Row],[Tmean]] + 237.3)))) / ((EToTable[[#This Row],[Tmean]] + 237.3) ^ 2), 4), "")</f>
-        <v>0.20019999999999999</v>
-      </c>
-      <c r="M10" s="29">
+        <v/>
+      </c>
+      <c r="M10" s="29" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[J]]), 0.409  * SIN( (2*PI()/365) * EToTable[[#This Row],[J]] - 1.39), "")</f>
-        <v>0.13972057295444912</v>
-      </c>
-      <c r="N10" s="30">
+        <v/>
+      </c>
+      <c r="N10" s="30" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[J]]), ROUND(1+0.033 * COS( (2*PI()/365) * EToTable[[#This Row],[J]]), 4), "")</f>
-        <v>0.99450000000000005</v>
+        <v/>
       </c>
       <c r="O10" s="30" t="str">
         <f>IF(AND(ISNUMBER(Latitude), ISNUMBER(EToTable[[#This Row],[Сана]])), ROUND((Latitude / 180) * PI(), 3), "")</f>
@@ -4495,41 +4489,41 @@
         <f xml:space="preserve"> IF(ISNUMBER(EToTable[[#This Row],[ωs]]), ( 24 / PI()) * EToTable[[#This Row],[ωs]], "")</f>
         <v/>
       </c>
-      <c r="S10" s="28">
+      <c r="S10" s="28" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]]), 0.6108 * EXP( 17.27 * EToTable[[#This Row],[Тмин
 (°С)]] / (EToTable[[#This Row],[Тмин
 (°С)]]+237.3)), "")</f>
-        <v>2.5023227554890153</v>
-      </c>
-      <c r="T10" s="28">
+        <v/>
+      </c>
+      <c r="T10" s="28" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[Тмакс
 (°С)]]), 0.6108 * EXP( 17.27 * EToTable[[#This Row],[Тмакс
 (°С)]] / (EToTable[[#This Row],[Тмакс
 (°С)]]+237.3)), "")</f>
-        <v>4.5439995866454055</v>
-      </c>
-      <c r="U10" s="28">
+        <v/>
+      </c>
+      <c r="U10" s="28" t="str">
         <f>IF(AND(ISNUMBER(EToTable[[#This Row],[e° (Tmin)]]), ISNUMBER(EToTable[[#This Row],[e° (Tmax)]])), (EToTable[[#This Row],[e° (Tmax)]]+EToTable[[#This Row],[e° (Tmin)]])/2, "")</f>
-        <v>3.5231611710672102</v>
-      </c>
-      <c r="V10" s="28">
+        <v/>
+      </c>
+      <c r="V10" s="28" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[Tdew]]), 0.6108 * EXP( 17.27 * (EToTable[[#This Row],[Tdew]]) / (EToTable[[#This Row],[Tdew]]+237.3)), "")</f>
-        <v>2.2111396340059919</v>
-      </c>
-      <c r="W10" s="30">
+        <v/>
+      </c>
+      <c r="W10" s="30" t="str">
         <f xml:space="preserve"> EToTable[[#This Row],[e° (Tdew)]]</f>
-        <v>2.2111396340059919</v>
-      </c>
-      <c r="X10" s="30">
+        <v/>
+      </c>
+      <c r="X10" s="30" t="str">
         <f>IF(AND(ISNUMBER(EToTable[[#This Row],[es]]), ISNUMBER(EToTable[[#This Row],[ea]])), EToTable[[#This Row],[es]]-EToTable[[#This Row],[ea]], "")</f>
-        <v>1.3120215370612183</v>
+        <v/>
       </c>
       <c r="Y10" s="28" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[Ra]]), (as+bs)*EToTable[[#This Row],[Ra]], "")</f>
         <v/>
       </c>
-      <c r="Z10" s="28" t="e">
+      <c r="Z10" s="28" t="str">
         <f>IF(AND(ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин
 (°С)]]), ISNUMBER(EToTable[[#This Row],[Тмакс
 (°С)]])), IF(ISNUMBER(EToTable[[#This Row],[Радиация
@@ -4537,7 +4531,7 @@
 (MJ/м2/к)]], IF( ISNUMBER(EToTable[[#This Row],[Қуёшли соат]]), (as + bs * MIN(EToTable[[#This Row],[Қуёшли соат]]/EToTable[[#This Row],[N]], 1))*EToTable[[#This Row],[Ra]], krs * SQRT( EToTable[[#This Row],[Тмакс
 (°С)]]-EToTable[[#This Row],[Тмин
 (°С)]] ) * EToTable[[#This Row],[Ra]] ) ), "")</f>
-        <v>#VALUE!</v>
+        <v/>
       </c>
       <c r="AA10" s="28" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[Rs]]), (1-albedo)*EToTable[[#This Row],[Rs]], "")</f>
@@ -4556,7 +4550,7 @@
         <f>IF(AND(ISNUMBER(EToTable[[#This Row],[Rns]]), ISNUMBER(EToTable[[#This Row],[Rnl]])), EToTable[[#This Row],[Rns]]-EToTable[[#This Row],[Rnl]], "")</f>
         <v/>
       </c>
-      <c r="AD10" s="30">
+      <c r="AD10" s="30" t="str">
         <f>IF(ISNUMBER(EToTable[[#This Row],[Сана]]), IF(ISNUMBER(EToTable[[#This Row],[Шамол
 (м/с)]]),
      IF(AnemometerHeight=2, MAX(EToTable[[#This Row],[Шамол
@@ -4564,7 +4558,7 @@
      MAX( EToTable[[#This Row],[Шамол
 (м/с)]] * 4.87 / LN(67.8 * AnemometerHeight - 5.42), 0.5)
 ), u2_default), "")</f>
-        <v>1.5</v>
+        <v/>
       </c>
       <c r="AE10" s="24" t="str">
         <f xml:space="preserve"> IF(AND(ISNUMBER(Latitude), ISNUMBER(Altitude), ISNUMBER(EToTable[[#This Row],[Сана]]), ISNUMBER(EToTable[[#This Row],[Тмин
@@ -5104,7 +5098,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="M26" sqref="M26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>